<commit_message>
test dati di mercato
</commit_message>
<xml_diff>
--- a/earlywarning-pom/Document/test/CORPORATE/test_nuovo_DdM.xlsx
+++ b/earlywarning-pom/Document/test/CORPORATE/test_nuovo_DdM.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilaria.cutano\Desktop\ISP\git\client-intesa\client-intesa\earlywarning-pom\Document\test\CORPORATE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tools\progetto Intesa\client-intesa\earlywarning-pom\Document\test\CORPORATE\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="126">
   <si>
     <t>BR170 - Distance to default S30</t>
   </si>
@@ -402,12 +402,15 @@
   </si>
   <si>
     <t>'S00'</t>
+  </si>
+  <si>
+    <t>non ci sono casi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -649,7 +652,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -963,22 +966,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.8984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.8984375" customWidth="1"/>
-    <col min="5" max="6" width="18.59765625" customWidth="1"/>
-    <col min="7" max="7" width="9.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.875" customWidth="1"/>
+    <col min="5" max="6" width="18.625" customWidth="1"/>
+    <col min="7" max="7" width="9.875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>55</v>
       </c>
@@ -992,7 +995,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>54</v>
       </c>
@@ -1009,7 +1012,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>54</v>
       </c>
@@ -1026,7 +1029,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>54</v>
       </c>
@@ -1043,7 +1046,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>54</v>
       </c>
@@ -1060,7 +1063,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>54</v>
       </c>
@@ -1080,7 +1083,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>54</v>
       </c>
@@ -1100,7 +1103,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>54</v>
       </c>
@@ -1120,7 +1123,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>54</v>
       </c>
@@ -1140,7 +1143,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>54</v>
       </c>
@@ -1151,7 +1154,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>54</v>
       </c>
@@ -1162,7 +1165,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>54</v>
       </c>
@@ -1173,7 +1176,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>54</v>
       </c>
@@ -1184,7 +1187,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>54</v>
       </c>
@@ -1195,7 +1198,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>54</v>
       </c>
@@ -1206,7 +1209,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>54</v>
       </c>
@@ -1217,7 +1220,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>54</v>
       </c>
@@ -1228,12 +1231,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
       <c r="B18" s="20"/>
       <c r="C18" s="21"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="1"/>
       <c r="C19" s="22" t="s">
@@ -1243,7 +1246,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C20" s="3" t="s">
         <v>38</v>
       </c>
@@ -1269,7 +1272,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>35</v>
       </c>
@@ -1301,7 +1304,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>35</v>
       </c>
@@ -1333,7 +1336,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>35</v>
       </c>
@@ -1365,10 +1368,10 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B24" s="13"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>37</v>
       </c>
@@ -1404,13 +1407,13 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>58</v>
       </c>
@@ -1418,7 +1421,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>60</v>
       </c>
@@ -1426,7 +1429,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>61</v>
       </c>
@@ -1434,7 +1437,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>62</v>
       </c>
@@ -1442,11 +1445,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
       <c r="B6" s="17"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>63</v>
       </c>
@@ -1454,7 +1457,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>64</v>
       </c>
@@ -1462,7 +1465,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>65</v>
       </c>
@@ -1470,7 +1473,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>66</v>
       </c>
@@ -1478,7 +1481,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>67</v>
       </c>
@@ -1496,23 +1499,23 @@
   <dimension ref="A1:H64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E50" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B61" sqref="B61"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.69921875" customWidth="1"/>
-    <col min="4" max="4" width="14.3984375" style="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.69921875" style="25"/>
+    <col min="2" max="2" width="13.75" customWidth="1"/>
+    <col min="4" max="4" width="14.375" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.75" style="25"/>
     <col min="6" max="6" width="56.5" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="56" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="66.69921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="66.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C1" s="26" t="s">
         <v>84</v>
       </c>
@@ -1532,9 +1535,12 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>123</v>
+      </c>
+      <c r="B2">
+        <v>17785168</v>
       </c>
       <c r="C2" s="27">
         <v>170</v>
@@ -1543,15 +1549,18 @@
         <v>87</v>
       </c>
       <c r="E2" s="29">
-        <v>0.78559999999999997</v>
+        <v>0.34339785</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
     </row>
-    <row r="3" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>123</v>
+      </c>
+      <c r="B3">
+        <v>48157162</v>
       </c>
       <c r="C3" s="27">
         <v>170</v>
@@ -1560,15 +1569,18 @@
         <v>89</v>
       </c>
       <c r="E3" s="29">
-        <v>0.79620000000000002</v>
+        <v>0.967481023133</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
     </row>
-    <row r="4" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>123</v>
+      </c>
+      <c r="B4">
+        <v>17824972</v>
       </c>
       <c r="C4" s="27">
         <v>171</v>
@@ -1577,15 +1589,18 @@
         <v>87</v>
       </c>
       <c r="E4" s="27">
-        <v>1.2678</v>
+        <v>2.0115282748999999</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
     </row>
-    <row r="5" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>123</v>
+      </c>
+      <c r="B5">
+        <v>48157162</v>
       </c>
       <c r="C5" s="27">
         <v>171</v>
@@ -1593,16 +1608,19 @@
       <c r="D5" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="E5" s="27">
-        <v>0.79620000000000002</v>
+      <c r="E5" s="29">
+        <v>0.967481023133</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>123</v>
+      </c>
+      <c r="B6">
+        <v>24596926</v>
       </c>
       <c r="C6" s="27">
         <v>171</v>
@@ -1611,15 +1629,18 @@
         <v>89</v>
       </c>
       <c r="E6" s="27">
-        <v>2.7052</v>
+        <v>2.6592996944</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>123</v>
+      </c>
+      <c r="B7">
+        <v>35993721</v>
       </c>
       <c r="C7" s="27">
         <v>171</v>
@@ -1627,16 +1648,19 @@
       <c r="D7" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="E7" s="27">
-        <v>0.78559999999999997</v>
+      <c r="E7" s="29">
+        <v>0.71354871696699995</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>123</v>
+      </c>
+      <c r="B8">
+        <v>24596926</v>
       </c>
       <c r="C8" s="27">
         <v>172</v>
@@ -1645,15 +1669,18 @@
         <v>87</v>
       </c>
       <c r="E8" s="27">
-        <v>2.6423000000000001</v>
+        <v>2.6592996944</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>123</v>
+      </c>
+      <c r="B9">
+        <v>54172736</v>
       </c>
       <c r="C9" s="27">
         <v>172</v>
@@ -1662,15 +1689,18 @@
         <v>87</v>
       </c>
       <c r="E9" s="27">
-        <v>4.2567000000000004</v>
+        <v>4.2055617217670003</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>123</v>
+      </c>
+      <c r="B10">
+        <v>70525969</v>
       </c>
       <c r="C10" s="27">
         <v>172</v>
@@ -1679,15 +1709,18 @@
         <v>87</v>
       </c>
       <c r="E10" s="27">
-        <v>5.1067</v>
+        <v>5.1261168302669997</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>123</v>
+      </c>
+      <c r="B11">
+        <v>48157162</v>
       </c>
       <c r="C11" s="27">
         <v>172</v>
@@ -1695,16 +1728,19 @@
       <c r="D11" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="E11" s="27">
-        <v>0.79620000000000002</v>
+      <c r="E11" s="29">
+        <v>0.967481023133</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>123</v>
+      </c>
+      <c r="B12">
+        <v>17824972</v>
       </c>
       <c r="C12" s="27">
         <v>172</v>
@@ -1713,15 +1749,18 @@
         <v>89</v>
       </c>
       <c r="E12" s="27">
-        <v>2.5522999999999998</v>
+        <v>2.0115282748999999</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>123</v>
+      </c>
+      <c r="B13">
+        <v>48523797</v>
       </c>
       <c r="C13" s="27">
         <v>173</v>
@@ -1730,15 +1769,18 @@
         <v>87</v>
       </c>
       <c r="E13" s="27">
-        <v>5.1866000000000003</v>
+        <v>5.2526539540670001</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>123</v>
+      </c>
+      <c r="B14">
+        <v>48215089</v>
       </c>
       <c r="C14" s="27">
         <v>173</v>
@@ -1747,15 +1789,18 @@
         <v>87</v>
       </c>
       <c r="E14" s="27">
-        <v>5.2568999999999999</v>
+        <v>5.2978484129999996</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>123</v>
+      </c>
+      <c r="B15">
+        <v>70525969</v>
       </c>
       <c r="C15" s="27">
         <v>173</v>
@@ -1764,15 +1809,18 @@
         <v>89</v>
       </c>
       <c r="E15" s="27">
-        <v>5.1669999999999998</v>
+        <v>5.1261168302669997</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>123</v>
+      </c>
+      <c r="B16">
+        <v>24596926</v>
       </c>
       <c r="C16" s="27">
         <v>173</v>
@@ -1781,13 +1829,13 @@
         <v>89</v>
       </c>
       <c r="E16" s="27">
-        <v>2.6423000000000001</v>
+        <v>2.6592996944</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>123</v>
       </c>
@@ -1807,7 +1855,7 @@
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>123</v>
       </c>
@@ -1827,7 +1875,7 @@
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>123</v>
       </c>
@@ -1847,7 +1895,7 @@
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>123</v>
       </c>
@@ -1867,7 +1915,7 @@
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>123</v>
       </c>
@@ -1887,7 +1935,7 @@
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>123</v>
       </c>
@@ -1907,7 +1955,7 @@
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>123</v>
       </c>
@@ -1927,7 +1975,7 @@
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>123</v>
       </c>
@@ -1947,7 +1995,7 @@
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>123</v>
       </c>
@@ -1967,7 +2015,7 @@
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>123</v>
       </c>
@@ -1987,7 +2035,7 @@
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>123</v>
       </c>
@@ -2007,7 +2055,7 @@
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>123</v>
       </c>
@@ -2027,7 +2075,7 @@
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>123</v>
       </c>
@@ -2047,7 +2095,7 @@
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>123</v>
       </c>
@@ -2067,7 +2115,7 @@
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>123</v>
       </c>
@@ -2087,7 +2135,7 @@
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>123</v>
       </c>
@@ -2107,7 +2155,7 @@
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>123</v>
       </c>
@@ -2127,7 +2175,7 @@
       </c>
       <c r="H33" s="10"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>123</v>
       </c>
@@ -2147,7 +2195,7 @@
       </c>
       <c r="H34" s="10"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>123</v>
       </c>
@@ -2167,7 +2215,7 @@
       </c>
       <c r="H35" s="10"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>123</v>
       </c>
@@ -2187,7 +2235,7 @@
       </c>
       <c r="H36" s="10"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>123</v>
       </c>
@@ -2207,7 +2255,7 @@
       </c>
       <c r="H37" s="10"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>123</v>
       </c>
@@ -2227,7 +2275,7 @@
       </c>
       <c r="H38" s="10"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>123</v>
       </c>
@@ -2247,7 +2295,7 @@
       </c>
       <c r="H39" s="10"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>123</v>
       </c>
@@ -2267,7 +2315,7 @@
       </c>
       <c r="H40" s="10"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>123</v>
       </c>
@@ -2287,7 +2335,7 @@
       </c>
       <c r="H41" s="10"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>123</v>
       </c>
@@ -2307,7 +2355,7 @@
       </c>
       <c r="H42" s="10"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>123</v>
       </c>
@@ -2327,7 +2375,7 @@
       </c>
       <c r="H43" s="10"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>123</v>
       </c>
@@ -2347,7 +2395,7 @@
       </c>
       <c r="H44" s="10"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>123</v>
       </c>
@@ -2367,7 +2415,7 @@
       </c>
       <c r="H45" s="10"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>123</v>
       </c>
@@ -2387,7 +2435,7 @@
       </c>
       <c r="H46" s="10"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>123</v>
       </c>
@@ -2407,7 +2455,7 @@
       </c>
       <c r="H47" s="10"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>123</v>
       </c>
@@ -2427,7 +2475,7 @@
       </c>
       <c r="H48" s="10"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>123</v>
       </c>
@@ -2447,7 +2495,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>123</v>
       </c>
@@ -2467,7 +2515,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>123</v>
       </c>
@@ -2487,7 +2535,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>123</v>
       </c>
@@ -2507,7 +2555,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>123</v>
       </c>
@@ -2527,7 +2575,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>123</v>
       </c>
@@ -2547,7 +2595,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>123</v>
       </c>
@@ -2567,7 +2615,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>123</v>
       </c>
@@ -2587,7 +2635,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>123</v>
       </c>
@@ -2607,7 +2655,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>123</v>
       </c>
@@ -2627,7 +2675,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>123</v>
       </c>
@@ -2647,7 +2695,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>123</v>
       </c>
@@ -2667,7 +2715,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>123</v>
       </c>
@@ -2687,7 +2735,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>123</v>
       </c>
@@ -2707,7 +2755,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>123</v>
       </c>
@@ -2727,7 +2775,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>123</v>
       </c>
@@ -2754,114 +2802,117 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S1048546"/>
+  <dimension ref="A1:T1048546"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E38" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26" style="25" customWidth="1"/>
-    <col min="3" max="3" width="10.59765625" style="25" customWidth="1"/>
-    <col min="4" max="19" width="9.19921875" style="25" customWidth="1"/>
+    <col min="2" max="2" width="17.375" style="25" customWidth="1"/>
+    <col min="3" max="3" width="26" style="25" customWidth="1"/>
+    <col min="4" max="4" width="10.625" style="25" customWidth="1"/>
+    <col min="5" max="20" width="9.25" style="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B1" s="22" t="s">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C1" s="22" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C2" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="D2" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="E2" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="F2" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="G2" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="H2" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="I2" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="J2" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="K2" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="K2" s="26" t="s">
+      <c r="L2" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="L2" s="26" t="s">
+      <c r="M2" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="M2" s="26" t="s">
+      <c r="N2" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="N2" s="26" t="s">
+      <c r="O2" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="O2" s="26" t="s">
+      <c r="P2" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="P2" s="26" t="s">
+      <c r="Q2" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="Q2" s="26" t="s">
+      <c r="R2" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="26" t="s">
+      <c r="S2" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="S2" s="26" t="s">
+      <c r="T2" s="26" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="25">
         <v>68658585</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="C3" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="D3" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="E3" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="E3" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="F3" s="36" t="s">
         <v>109</v>
       </c>
       <c r="G3" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="H3" s="42" t="s">
-        <v>108</v>
-      </c>
-      <c r="I3" s="36" t="s">
+      <c r="H3" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="I3" s="42" t="s">
         <v>108</v>
       </c>
       <c r="J3" s="36" t="s">
         <v>108</v>
       </c>
       <c r="K3" s="36" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L3" s="36" t="s">
         <v>109</v>
@@ -2887,23 +2938,26 @@
       <c r="S3" s="36" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="T3" s="36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" s="25">
         <v>17785168</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="C4" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="D4" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="D4" s="42" t="s">
+      <c r="E4" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="E4" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="F4" s="36" t="s">
         <v>109</v>
       </c>
@@ -2946,20 +3000,23 @@
       <c r="S4" s="36" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="T4" s="36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" s="25">
         <v>18011915</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="C5" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="D5" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="D5" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="E5" s="36" t="s">
         <v>109</v>
       </c>
@@ -2969,18 +3026,18 @@
       <c r="G5" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="H5" s="42" t="s">
+      <c r="H5" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="I5" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="I5" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="J5" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="K5" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="K5" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="L5" s="36" t="s">
         <v>109</v>
       </c>
@@ -2991,11 +3048,11 @@
         <v>109</v>
       </c>
       <c r="O5" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="P5" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="P5" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="Q5" s="36" t="s">
         <v>109</v>
       </c>
@@ -3005,26 +3062,29 @@
       <c r="S5" s="36" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="T5" s="36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" s="25">
         <v>48157162</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="C6" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="D6" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="D6" s="36" t="s">
-        <v>109</v>
-      </c>
-      <c r="E6" s="42" t="s">
+      <c r="E6" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="F6" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="F6" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="G6" s="36" t="s">
         <v>109</v>
       </c>
@@ -3032,11 +3092,11 @@
         <v>109</v>
       </c>
       <c r="I6" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="J6" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="J6" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="K6" s="36" t="s">
         <v>109</v>
       </c>
@@ -3064,35 +3124,38 @@
       <c r="S6" s="36" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="T6" s="36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" s="25">
         <v>74631051</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="C7" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="D7" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="D7" s="36" t="s">
-        <v>109</v>
-      </c>
-      <c r="E7" s="42" t="s">
+      <c r="E7" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="F7" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="F7" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="G7" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="H7" s="42" t="s">
+      <c r="H7" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="I7" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="I7" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="J7" s="36" t="s">
         <v>109</v>
       </c>
@@ -3112,31 +3175,34 @@
         <v>109</v>
       </c>
       <c r="P7" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q7" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="Q7" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="R7" s="36" t="s">
         <v>109</v>
       </c>
       <c r="S7" s="36" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="T7" s="36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B8" s="25">
         <v>59734615</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="C8" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="D8" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="D8" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="E8" s="36" t="s">
         <v>109</v>
       </c>
@@ -3146,15 +3212,15 @@
       <c r="G8" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="H8" s="42" t="s">
+      <c r="H8" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="I8" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="I8" s="36" t="s">
+      <c r="J8" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="J8" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="K8" s="36" t="s">
         <v>109</v>
       </c>
@@ -3171,37 +3237,43 @@
         <v>109</v>
       </c>
       <c r="P8" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q8" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="Q8" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="R8" s="36" t="s">
         <v>109</v>
       </c>
       <c r="S8" s="36" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B9" s="27" t="s">
+      <c r="T8" s="36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" s="25">
+        <v>35924655</v>
+      </c>
+      <c r="C9" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="D9" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="D9" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="E9" s="36" t="s">
         <v>109</v>
       </c>
       <c r="F9" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="G9" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="G9" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="H9" s="36" t="s">
         <v>109</v>
       </c>
@@ -3209,11 +3281,11 @@
         <v>109</v>
       </c>
       <c r="J9" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="K9" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="K9" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="L9" s="36" t="s">
         <v>109</v>
       </c>
@@ -3238,26 +3310,32 @@
       <c r="S9" s="36" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B10" s="27" t="s">
+      <c r="T9" s="36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" s="25">
+        <v>54247107</v>
+      </c>
+      <c r="C10" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="D10" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="D10" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="E10" s="36" t="s">
         <v>109</v>
       </c>
       <c r="F10" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="G10" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="G10" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="H10" s="36" t="s">
         <v>109</v>
       </c>
@@ -3294,17 +3372,23 @@
       <c r="S10" s="36" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B11" s="27" t="s">
+      <c r="T10" s="36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11" s="25">
+        <v>53805873</v>
+      </c>
+      <c r="C11" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="D11" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="D11" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="E11" s="36" t="s">
         <v>109</v>
       </c>
@@ -3321,11 +3405,11 @@
         <v>109</v>
       </c>
       <c r="J11" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="K11" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="K11" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="L11" s="36" t="s">
         <v>109</v>
       </c>
@@ -3350,26 +3434,32 @@
       <c r="S11" s="36" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B12" s="27" t="s">
+      <c r="T11" s="36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B12" s="25">
+        <v>35924655</v>
+      </c>
+      <c r="C12" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="D12" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="D12" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="E12" s="36" t="s">
         <v>109</v>
       </c>
       <c r="F12" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="G12" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="G12" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="H12" s="36" t="s">
         <v>109</v>
       </c>
@@ -3377,11 +3467,11 @@
         <v>109</v>
       </c>
       <c r="J12" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="K12" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="K12" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="L12" s="36" t="s">
         <v>109</v>
       </c>
@@ -3406,17 +3496,23 @@
       <c r="S12" s="36" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B13" s="27" t="s">
+      <c r="T12" s="36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>123</v>
+      </c>
+      <c r="B13" s="25">
+        <v>18001630</v>
+      </c>
+      <c r="C13" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="D13" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="D13" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="E13" s="36" t="s">
         <v>109</v>
       </c>
@@ -3424,11 +3520,11 @@
         <v>109</v>
       </c>
       <c r="G13" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="H13" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="H13" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="I13" s="36" t="s">
         <v>109</v>
       </c>
@@ -3436,11 +3532,11 @@
         <v>109</v>
       </c>
       <c r="K13" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="L13" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="L13" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="M13" s="36" t="s">
         <v>109</v>
       </c>
@@ -3462,17 +3558,23 @@
       <c r="S13" s="36" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B14" s="27" t="s">
+      <c r="T13" s="36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>123</v>
+      </c>
+      <c r="B14" s="25">
+        <v>28414322</v>
+      </c>
+      <c r="C14" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="D14" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="D14" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="E14" s="36" t="s">
         <v>109</v>
       </c>
@@ -3480,11 +3582,11 @@
         <v>109</v>
       </c>
       <c r="G14" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="H14" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="H14" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="I14" s="36" t="s">
         <v>109</v>
       </c>
@@ -3518,17 +3620,23 @@
       <c r="S14" s="36" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B15" s="27" t="s">
+      <c r="T14" s="36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>123</v>
+      </c>
+      <c r="B15" s="25">
+        <v>36054664</v>
+      </c>
+      <c r="C15" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="D15" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="D15" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="E15" s="36" t="s">
         <v>109</v>
       </c>
@@ -3548,11 +3656,11 @@
         <v>109</v>
       </c>
       <c r="K15" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="L15" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="L15" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="M15" s="36" t="s">
         <v>109</v>
       </c>
@@ -3574,20 +3682,26 @@
       <c r="S15" s="36" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B16" s="27" t="s">
+      <c r="T15" s="36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>123</v>
+      </c>
+      <c r="B16" s="25">
+        <v>58954695</v>
+      </c>
+      <c r="C16" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="D16" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="D16" s="36" t="s">
+      <c r="E16" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="E16" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="F16" s="36" t="s">
         <v>109</v>
       </c>
@@ -3607,11 +3721,11 @@
         <v>109</v>
       </c>
       <c r="L16" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="M16" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="M16" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="N16" s="36" t="s">
         <v>109</v>
       </c>
@@ -3630,17 +3744,23 @@
       <c r="S16" s="36" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B17" s="27" t="s">
+      <c r="T16" s="36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>123</v>
+      </c>
+      <c r="B17" s="25">
+        <v>53805873</v>
+      </c>
+      <c r="C17" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="D17" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="D17" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="E17" s="36" t="s">
         <v>109</v>
       </c>
@@ -3666,11 +3786,11 @@
         <v>109</v>
       </c>
       <c r="M17" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="N17" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="N17" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="O17" s="36" t="s">
         <v>109</v>
       </c>
@@ -3684,19 +3804,25 @@
         <v>109</v>
       </c>
       <c r="S17" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="T17" s="36" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B18" s="27" t="s">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>123</v>
+      </c>
+      <c r="B18" s="25">
+        <v>17996707</v>
+      </c>
+      <c r="C18" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="C18" s="28" t="s">
+      <c r="D18" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="D18" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="E18" s="36" t="s">
         <v>109</v>
       </c>
@@ -3725,11 +3851,11 @@
         <v>109</v>
       </c>
       <c r="N18" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="O18" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="O18" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="P18" s="36" t="s">
         <v>109</v>
       </c>
@@ -3742,17 +3868,23 @@
       <c r="S18" s="36" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B19" s="27" t="s">
+      <c r="T18" s="36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>123</v>
+      </c>
+      <c r="B19" s="25">
+        <v>17985417</v>
+      </c>
+      <c r="C19" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="D19" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="D19" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="E19" s="36" t="s">
         <v>109</v>
       </c>
@@ -3763,11 +3895,11 @@
         <v>109</v>
       </c>
       <c r="H19" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="I19" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="I19" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="J19" s="36" t="s">
         <v>109</v>
       </c>
@@ -3784,11 +3916,11 @@
         <v>109</v>
       </c>
       <c r="O19" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="P19" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="P19" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="Q19" s="36" t="s">
         <v>109</v>
       </c>
@@ -3798,17 +3930,23 @@
       <c r="S19" s="36" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B20" s="27" t="s">
+      <c r="T19" s="36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>123</v>
+      </c>
+      <c r="B20" s="25">
+        <v>73810233</v>
+      </c>
+      <c r="C20" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="C20" s="28" t="s">
+      <c r="D20" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="D20" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="E20" s="36" t="s">
         <v>109</v>
       </c>
@@ -3843,28 +3981,34 @@
         <v>109</v>
       </c>
       <c r="P20" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q20" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="Q20" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="R20" s="36" t="s">
         <v>109</v>
       </c>
       <c r="S20" s="36" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B21" s="27" t="s">
+      <c r="T20" s="36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>123</v>
+      </c>
+      <c r="B21" s="25">
+        <v>68640807</v>
+      </c>
+      <c r="C21" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="D21" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="D21" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="E21" s="36" t="s">
         <v>109</v>
       </c>
@@ -3902,25 +4046,31 @@
         <v>109</v>
       </c>
       <c r="Q21" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="R21" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="R21" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="S21" s="36" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B22" s="27" t="s">
+      <c r="T21" s="36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>123</v>
+      </c>
+      <c r="B22" s="25">
+        <v>18011825</v>
+      </c>
+      <c r="C22" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="C22" s="28" t="s">
+      <c r="D22" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="D22" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="E22" s="36" t="s">
         <v>109</v>
       </c>
@@ -3961,22 +4111,28 @@
         <v>109</v>
       </c>
       <c r="R22" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="S22" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="S22" s="36" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B23" s="27" t="s">
+      <c r="T22" s="36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>123</v>
+      </c>
+      <c r="B23" s="25">
+        <v>49969769</v>
+      </c>
+      <c r="C23" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="C23" s="28" t="s">
+      <c r="D23" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="D23" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="E23" s="36" t="s">
         <v>109</v>
       </c>
@@ -4020,14 +4176,16 @@
         <v>109</v>
       </c>
       <c r="S23" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="T23" s="42" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B25" s="35" t="s">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C25" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="C25"/>
       <c r="D25"/>
       <c r="E25"/>
       <c r="F25"/>
@@ -4044,64 +4202,68 @@
       <c r="Q25"/>
       <c r="R25"/>
       <c r="S25"/>
-    </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B26" s="37" t="s">
+      <c r="T25"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C26" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="37" t="s">
+      <c r="D26" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="D26" s="37" t="s">
+      <c r="E26" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="E26" s="37" t="s">
+      <c r="F26" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="F26" s="37" t="s">
+      <c r="G26" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="G26" s="37" t="s">
+      <c r="H26" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="H26" s="37" t="s">
+      <c r="I26" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="I26" s="37" t="s">
+      <c r="J26" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="J26" s="37" t="s">
+      <c r="K26" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="K26" s="37" t="s">
+      <c r="L26" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="L26" s="37" t="s">
+      <c r="M26" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="M26" s="37" t="s">
+      <c r="N26" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="N26" s="37" t="s">
+      <c r="O26" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="O26" s="37" t="s">
+      <c r="P26" s="37" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B27" s="38" t="s">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>123</v>
+      </c>
+      <c r="B27" s="25">
+        <v>52832541</v>
+      </c>
+      <c r="C27" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="C27" s="36" t="s">
+      <c r="D27" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="D27" s="36" t="s">
+      <c r="E27" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="E27" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="F27" s="36" t="s">
         <v>109</v>
       </c>
@@ -4132,23 +4294,29 @@
       <c r="O27" s="36" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B28" s="38" t="s">
+      <c r="P27" s="36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>123</v>
+      </c>
+      <c r="B28" s="25">
+        <v>74754023</v>
+      </c>
+      <c r="C28" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="C28" s="36" t="s">
+      <c r="D28" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="D28" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="E28" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="F28" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="F28" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="G28" s="36" t="s">
         <v>109</v>
       </c>
@@ -4176,26 +4344,32 @@
       <c r="O28" s="36" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B29" s="38" t="s">
+      <c r="P28" s="36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>123</v>
+      </c>
+      <c r="B29" s="25">
+        <v>49951845</v>
+      </c>
+      <c r="C29" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="C29" s="36" t="s">
+      <c r="D29" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="D29" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="E29" s="36" t="s">
         <v>109</v>
       </c>
       <c r="F29" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="G29" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="G29" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="H29" s="36" t="s">
         <v>109</v>
       </c>
@@ -4206,11 +4380,11 @@
         <v>109</v>
       </c>
       <c r="K29" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="L29" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="L29" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="M29" s="36" t="s">
         <v>109</v>
       </c>
@@ -4220,17 +4394,23 @@
       <c r="O29" s="36" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="30" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B30" s="38" t="s">
+      <c r="P29" s="36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>123</v>
+      </c>
+      <c r="B30" s="25">
+        <v>18011279</v>
+      </c>
+      <c r="C30" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="C30" s="36" t="s">
+      <c r="D30" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="D30" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="E30" s="36" t="s">
         <v>109</v>
       </c>
@@ -4238,11 +4418,11 @@
         <v>109</v>
       </c>
       <c r="G30" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="H30" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="H30" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="I30" s="36" t="s">
         <v>109</v>
       </c>
@@ -4264,17 +4444,23 @@
       <c r="O30" s="36" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="31" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B31" s="38" t="s">
+      <c r="P30" s="36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>123</v>
+      </c>
+      <c r="B31" s="25">
+        <v>18005540</v>
+      </c>
+      <c r="C31" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="C31" s="36" t="s">
+      <c r="D31" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="D31" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="E31" s="36" t="s">
         <v>109</v>
       </c>
@@ -4285,11 +4471,11 @@
         <v>109</v>
       </c>
       <c r="H31" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="I31" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="I31" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="J31" s="36" t="s">
         <v>109</v>
       </c>
@@ -4308,17 +4494,23 @@
       <c r="O31" s="36" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="32" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B32" s="38" t="s">
+      <c r="P31" s="36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>123</v>
+      </c>
+      <c r="B32" s="25">
+        <v>48239421</v>
+      </c>
+      <c r="C32" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="C32" s="36" t="s">
+      <c r="D32" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="D32" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="E32" s="36" t="s">
         <v>109</v>
       </c>
@@ -4332,11 +4524,11 @@
         <v>109</v>
       </c>
       <c r="I32" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="J32" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="J32" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="K32" s="36" t="s">
         <v>109</v>
       </c>
@@ -4350,19 +4542,25 @@
         <v>109</v>
       </c>
       <c r="O32" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="P32" s="36" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B33" s="38" t="s">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>123</v>
+      </c>
+      <c r="B33" s="25">
+        <v>67566239</v>
+      </c>
+      <c r="C33" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="C33" s="36" t="s">
+      <c r="D33" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="D33" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="E33" s="36" t="s">
         <v>109</v>
       </c>
@@ -4379,11 +4577,11 @@
         <v>109</v>
       </c>
       <c r="J33" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="K33" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="K33" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="L33" s="36" t="s">
         <v>109</v>
       </c>
@@ -4396,20 +4594,26 @@
       <c r="O33" s="36" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B34" s="38" t="s">
+      <c r="P33" s="36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>123</v>
+      </c>
+      <c r="B34" s="25">
+        <v>68633431</v>
+      </c>
+      <c r="C34" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="C34" s="36" t="s">
+      <c r="D34" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="D34" s="36" t="s">
+      <c r="E34" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="E34" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="F34" s="36" t="s">
         <v>109</v>
       </c>
@@ -4426,11 +4630,11 @@
         <v>109</v>
       </c>
       <c r="K34" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="L34" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="L34" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="M34" s="36" t="s">
         <v>109</v>
       </c>
@@ -4440,17 +4644,23 @@
       <c r="O34" s="36" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B35" s="38" t="s">
+      <c r="P34" s="36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>123</v>
+      </c>
+      <c r="B35" s="25">
+        <v>24857039</v>
+      </c>
+      <c r="C35" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="C35" s="36" t="s">
+      <c r="D35" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="D35" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="E35" s="36" t="s">
         <v>109</v>
       </c>
@@ -4473,28 +4683,34 @@
         <v>109</v>
       </c>
       <c r="L35" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="M35" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="M35" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="N35" s="36" t="s">
         <v>109</v>
       </c>
       <c r="O35" s="36" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B36" s="38" t="s">
+      <c r="P35" s="36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>123</v>
+      </c>
+      <c r="B36" s="25">
+        <v>18009632</v>
+      </c>
+      <c r="C36" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="C36" s="36" t="s">
+      <c r="D36" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="D36" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="E36" s="36" t="s">
         <v>109</v>
       </c>
@@ -4520,25 +4736,31 @@
         <v>109</v>
       </c>
       <c r="M36" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="N36" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="N36" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="O36" s="36" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B37" s="38" t="s">
+      <c r="P36" s="36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>123</v>
+      </c>
+      <c r="B37" s="25">
+        <v>67821881</v>
+      </c>
+      <c r="C37" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="C37" s="36" t="s">
+      <c r="D37" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="D37" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="E37" s="36" t="s">
         <v>109</v>
       </c>
@@ -4567,22 +4789,28 @@
         <v>109</v>
       </c>
       <c r="N37" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="O37" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="O37" s="36" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B38" s="38" t="s">
+      <c r="P37" s="36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>123</v>
+      </c>
+      <c r="B38" s="25">
+        <v>36060393</v>
+      </c>
+      <c r="C38" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="C38" s="36" t="s">
+      <c r="D38" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="D38" s="36" t="s">
-        <v>109</v>
-      </c>
       <c r="E38" s="36" t="s">
         <v>109</v>
       </c>
@@ -4614,12 +4842,14 @@
         <v>109</v>
       </c>
       <c r="O38" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="P38" s="36" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B39" s="41"/>
-      <c r="C39" s="39"/>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C39" s="41"/>
       <c r="D39" s="39"/>
       <c r="E39" s="39"/>
       <c r="F39" s="39"/>
@@ -4632,25 +4862,28 @@
       <c r="M39" s="39"/>
       <c r="N39" s="39"/>
       <c r="O39" s="39"/>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B41" s="37" t="s">
+      <c r="P39" s="39"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C41" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="C41" s="37" t="s">
+      <c r="D41" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="D41" s="37" t="s">
+      <c r="E41" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="E41" s="37" t="s">
+      <c r="F41" s="37" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A42" s="40"/>
-      <c r="B42" s="28" t="s">
-        <v>110</v>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>123</v>
+      </c>
+      <c r="B42" s="40">
+        <v>52832541</v>
       </c>
       <c r="C42" s="28" t="s">
         <v>110</v>
@@ -4661,71 +4894,93 @@
       <c r="E42" s="28" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A43" s="40"/>
-      <c r="B43" s="28" t="s">
+      <c r="F42" s="28" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>123</v>
+      </c>
+      <c r="B43" s="40">
+        <v>35993721</v>
+      </c>
+      <c r="C43" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="C43" s="36" t="s">
+      <c r="D43" s="36" t="s">
         <v>112</v>
-      </c>
-      <c r="D43" s="28" t="s">
-        <v>111</v>
       </c>
       <c r="E43" s="28" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A44" s="40"/>
-      <c r="B44" s="28" t="s">
+      <c r="F43" s="28" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B44" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="C44" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="C44" s="36" t="s">
+      <c r="D44" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="D44" s="28" t="s">
+      <c r="E44" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="E44" s="36" t="s">
+      <c r="F44" s="36" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A45" s="40"/>
-      <c r="B45" s="36" t="s">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>123</v>
+      </c>
+      <c r="B45" s="40">
+        <v>67871336</v>
+      </c>
+      <c r="C45" s="36" t="s">
         <v>113</v>
-      </c>
-      <c r="C45" s="28" t="s">
-        <v>124</v>
       </c>
       <c r="D45" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="E45" s="36" t="s">
+      <c r="E45" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="F45" s="36" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A46" s="40"/>
-      <c r="B46" s="28" t="s">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>123</v>
+      </c>
+      <c r="B46" s="40">
+        <v>49847461</v>
+      </c>
+      <c r="C46" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="C46" s="36" t="s">
+      <c r="D46" s="36" t="s">
         <v>124</v>
       </c>
-      <c r="D46" s="28" t="s">
+      <c r="E46" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="E46" s="36" t="s">
+      <c r="F46" s="36" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A47" s="40"/>
-      <c r="B47" s="36" t="s">
-        <v>112</v>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>123</v>
+      </c>
+      <c r="B47" s="40">
+        <v>17996256</v>
       </c>
       <c r="C47" s="36" t="s">
         <v>112</v>
@@ -4736,38 +4991,56 @@
       <c r="E47" s="36" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B48" s="36" t="s">
+      <c r="F47" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="C48" s="43" t="s">
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>123</v>
+      </c>
+      <c r="B48" s="25">
+        <v>17956132</v>
+      </c>
+      <c r="C48" s="36" t="s">
         <v>112</v>
       </c>
       <c r="D48" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="E48" s="44" t="s">
+      <c r="E48" s="43" t="s">
+        <v>112</v>
+      </c>
+      <c r="F48" s="44" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B49" s="28" t="s">
-        <v>111</v>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>123</v>
+      </c>
+      <c r="B49" s="25">
+        <v>36034521</v>
       </c>
       <c r="C49" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="D49" s="36" t="s">
+      <c r="D49" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="E49" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="E49" s="28" t="s">
+      <c r="F49" s="28" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B50" s="28" t="s">
-        <v>124</v>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>123</v>
+      </c>
+      <c r="B50" s="25">
+        <v>46919274</v>
       </c>
       <c r="C50" s="28" t="s">
         <v>124</v>
@@ -4778,66 +5051,96 @@
       <c r="E50" s="28" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B51" s="36" t="s">
-        <v>111</v>
+      <c r="F50" s="28" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>123</v>
+      </c>
+      <c r="B51" s="25">
+        <v>26855585</v>
       </c>
       <c r="C51" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="D51" s="28" t="s">
-        <v>124</v>
+      <c r="D51" s="36" t="s">
+        <v>111</v>
       </c>
       <c r="E51" s="28" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B52" s="36" t="s">
+      <c r="F51" s="28" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>123</v>
+      </c>
+      <c r="B52" s="25">
+        <v>35133640</v>
+      </c>
+      <c r="C52" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="C52" s="28" t="s">
+      <c r="D52" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="D52" s="36" t="s">
+      <c r="E52" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="E52" s="28" t="s">
+      <c r="F52" s="28" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B53" s="36" t="s">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>123</v>
+      </c>
+      <c r="B53" s="25">
+        <v>36054664</v>
+      </c>
+      <c r="C53" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="C53" s="36" t="s">
+      <c r="D53" s="36" t="s">
         <v>113</v>
-      </c>
-      <c r="D53" s="36" t="s">
-        <v>111</v>
       </c>
       <c r="E53" s="36" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B54" s="36" t="s">
+      <c r="F53" s="36" t="s">
         <v>111</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>123</v>
+      </c>
+      <c r="B54" s="25">
+        <v>70525969</v>
       </c>
       <c r="C54" s="36" t="s">
         <v>111</v>
       </c>
       <c r="D54" s="36" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E54" s="36" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B55" s="36" t="s">
+      <c r="F54" s="36" t="s">
         <v>113</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>123</v>
+      </c>
+      <c r="B55" s="25">
+        <v>27586308</v>
       </c>
       <c r="C55" s="36" t="s">
         <v>113</v>
@@ -4848,9 +5151,12 @@
       <c r="E55" s="36" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="1048546" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C1048546" s="34"/>
+      <c r="F55" s="36" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="1048546" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D1048546" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>